<commit_message>
Add beautiful bif diagrams
</commit_message>
<xml_diff>
--- a/data_process/data.xlsx
+++ b/data_process/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chua's_curcuit\data_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B590A6-B962-49E7-BC15-CF75D36BF77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EAC36F-E7CB-4E1B-8BDD-126A3D2788B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,15 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>Переход БПЦ к ДПА</t>
   </si>
   <si>
     <t>Переход от ДПА к АР</t>
-  </si>
-  <si>
-    <t>Переход от АP к ДПЦ</t>
   </si>
   <si>
     <t>Переход от ДПЦ к МПЦ</t>
@@ -118,9 +115,6 @@
     <t>Diameter</t>
   </si>
   <si>
-    <t>Пересчитанные сопротивления</t>
-  </si>
-  <si>
     <t>Для схемы</t>
   </si>
   <si>
@@ -174,12 +168,6 @@
   <si>
     <t>Переход в финальный БПЦ</t>
   </si>
-  <si>
-    <t>Теория</t>
-  </si>
-  <si>
-    <t>Эксперимент</t>
-  </si>
 </sst>
 </file>
 
@@ -216,12 +204,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -236,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -244,6 +238,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -262,1086 +257,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>БПЦ к ДПА</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$A$18:$A$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.3000000000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.2400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2200000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$B$18:$B$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.15</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.9600000000000009</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.5500000000000007</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F38B-4FF7-969C-E1C5A1267E02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>ДПА к АР</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$C$18:$C$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1.27</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3800000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.48</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5500000000000003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.5700000000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.5100000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$D$18:$D$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>7.93</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.76</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.66</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.09</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F38B-4FF7-969C-E1C5A1267E02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>АР к ДПЦ</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$E$18:$E$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.52</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6300000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.58</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4300000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3600000000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$F$18:$F$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>7.52</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.27</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.52</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.1099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.6400000000000006</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F38B-4FF7-969C-E1C5A1267E02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>ДПЦ к МПЦ</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$G$18:$G$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.6400000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.58</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5500000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.4000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.21</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.1100000000000003</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3000000000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$H$18:$H$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.98</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.5500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.55</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.88</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.3599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.88</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.58</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.81</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F38B-4FF7-969C-E1C5A1267E02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>МПЦ к точке</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$I$18:$I$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.7000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6100000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5300000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.23</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$J$18:$J$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.1099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.74</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.55</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.8600000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.1900000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.0300000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-F38B-4FF7-969C-E1C5A1267E02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>точка к МПЦ</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$K$18:$K$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.46</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1700000000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5300000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6600000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$L$18:$L$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.1400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2899999999999991</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.3399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0399999999999991</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.97000000000000064</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.90000000000000036</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-F38B-4FF7-969C-E1C5A1267E02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>МПЦ к БПЦ</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$M$18:$M$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1.75</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6400000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.52</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1900000000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.02</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.80000000000000027</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.66999999999999993</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$N$18:$N$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.74000000000000021</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.66999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.66000000000000014</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.64000000000000057</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.60999999999999943</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5600000000000005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5600000000000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.5600000000000005</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-F38B-4FF7-969C-E1C5A1267E02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:v>БПЦ к МПЦ</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$O$18:$O$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1.7000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1900000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.99000000000000021</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.80000000000000027</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.70000000000000018</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.49000000000000021</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$P$18:$P$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.11999999999999922</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.11999999999999922</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.11999999999999922</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.13000000000000078</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.11999999999999922</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.11999999999999922</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.11999999999999922</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.11999999999999922</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-F38B-4FF7-969C-E1C5A1267E02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:v>БПЦ к МПЦ</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$Q$18:$Q$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.0500000000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95000000000000018</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.8400000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.74000000000000021</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.62000000000000011</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Состояние системы'!$R$18:$R$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4.5999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.17</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.09</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8200000000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-F38B-4FF7-969C-E1C5A1267E02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1921234191"/>
-        <c:axId val="1921222671"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1921234191"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1921222671"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1921222671"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1921234191"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
@@ -2741,7 +1656,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
@@ -3156,7 +2071,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
@@ -3640,46 +2555,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5228,572 +4103,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>69231</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>4535</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>169659</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>132698</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>668215</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>175846</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Диаграмма 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23BB6D6D-760F-F2C4-1B39-5D424E13D684}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>825826</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>16282</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>509301</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>121790</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>720968</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>37123</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5812,7 +4135,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6104,10 +4427,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AH59"/>
+  <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="72" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="72" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6135,90 +4458,81 @@
         <v>6</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="O2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="U2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" t="s">
         <v>42</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AA2" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>45</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG2" t="s">
         <v>47</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
@@ -6235,88 +4549,82 @@
         <v>2.0699999999999998</v>
       </c>
       <c r="E3" s="1">
-        <v>3.18</v>
+        <v>3.06</v>
       </c>
       <c r="F3" s="1">
-        <v>2.48</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>3.06</v>
+        <v>3</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1">
+        <v>3.24</v>
+      </c>
+      <c r="J3" s="1">
+        <v>8.86</v>
+      </c>
+      <c r="K3" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="L3" s="1">
+        <v>9.26</v>
+      </c>
+      <c r="M3" s="1">
         <v>3</v>
       </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>3.24</v>
-      </c>
-      <c r="L3" s="1">
-        <v>8.86</v>
-      </c>
-      <c r="M3" s="1">
-        <v>2.95</v>
-      </c>
       <c r="N3" s="1">
-        <v>9.26</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="O3" s="1">
-        <v>3</v>
+        <v>3.65</v>
       </c>
       <c r="P3" s="1">
-        <v>9.8800000000000008</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>3.65</v>
-      </c>
-      <c r="R3" s="1">
         <v>5.4</v>
       </c>
       <c r="U3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V3" t="s">
         <v>8</v>
       </c>
-      <c r="V3" t="s">
-        <v>9</v>
-      </c>
       <c r="W3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" t="s">
         <v>8</v>
       </c>
-      <c r="X3" t="s">
-        <v>9</v>
-      </c>
       <c r="Y3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" t="s">
-        <v>9</v>
-      </c>
       <c r="AA3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB3" t="s">
         <v>8</v>
       </c>
-      <c r="AB3" t="s">
-        <v>9</v>
-      </c>
       <c r="AC3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD3" t="s">
         <v>8</v>
       </c>
-      <c r="AD3" t="s">
-        <v>9</v>
-      </c>
       <c r="AE3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF3" t="s">
         <v>8</v>
       </c>
-      <c r="AF3" t="s">
-        <v>9</v>
-      </c>
       <c r="AG3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH3" t="s">
         <v>8</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
@@ -6333,45 +4641,39 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="E4" s="1">
-        <v>3.07</v>
+        <v>3.12</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="G4" s="1">
-        <v>3.12</v>
+        <v>3.09</v>
       </c>
       <c r="H4" s="1">
-        <v>1.02</v>
+        <v>2.89</v>
       </c>
       <c r="I4" s="1">
-        <v>3.09</v>
+        <v>3.53</v>
       </c>
       <c r="J4" s="1">
-        <v>2.89</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="K4" s="1">
-        <v>3.53</v>
+        <v>3.06</v>
       </c>
       <c r="L4" s="1">
-        <v>8.7100000000000009</v>
+        <v>9.33</v>
       </c>
       <c r="M4" s="1">
-        <v>3.06</v>
+        <v>3.1</v>
       </c>
       <c r="N4" s="1">
-        <v>9.33</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="O4" s="1">
-        <v>3.1</v>
+        <v>3.75</v>
       </c>
       <c r="P4" s="1">
-        <v>9.8800000000000008</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>3.75</v>
-      </c>
-      <c r="R4" s="1">
         <v>6.83</v>
       </c>
       <c r="U4">
@@ -6431,45 +4733,39 @@
         <v>2.34</v>
       </c>
       <c r="E5" s="1">
-        <v>3.12</v>
+        <v>3.15</v>
       </c>
       <c r="F5" s="1">
-        <v>0.73</v>
+        <v>1.45</v>
       </c>
       <c r="G5" s="1">
-        <v>3.15</v>
+        <v>3.17</v>
       </c>
       <c r="H5" s="1">
-        <v>1.45</v>
+        <v>3.26</v>
       </c>
       <c r="I5" s="1">
-        <v>3.17</v>
+        <v>3.35</v>
       </c>
       <c r="J5" s="1">
-        <v>3.26</v>
+        <v>8.66</v>
       </c>
       <c r="K5" s="1">
-        <v>3.35</v>
+        <v>3.18</v>
       </c>
       <c r="L5" s="1">
-        <v>8.66</v>
+        <v>9.34</v>
       </c>
       <c r="M5" s="1">
-        <v>3.18</v>
+        <v>3.3</v>
       </c>
       <c r="N5" s="1">
-        <v>9.34</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="O5" s="1">
-        <v>3.3</v>
+        <v>3.86</v>
       </c>
       <c r="P5" s="1">
-        <v>9.8800000000000008</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>3.86</v>
-      </c>
-      <c r="R5" s="1">
         <v>7</v>
       </c>
       <c r="U5">
@@ -6529,45 +4825,39 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E6" s="1">
-        <v>3.23</v>
+        <v>3.2</v>
       </c>
       <c r="F6" s="1">
-        <v>2.48</v>
+        <v>2.25</v>
       </c>
       <c r="G6" s="1">
-        <v>3.2</v>
+        <v>3.26</v>
       </c>
       <c r="H6" s="1">
-        <v>2.25</v>
+        <v>4.45</v>
       </c>
       <c r="I6" s="1">
+        <v>3.17</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="K6" s="1">
         <v>3.26</v>
       </c>
-      <c r="J6" s="1">
-        <v>4.45</v>
-      </c>
-      <c r="K6" s="1">
-        <v>3.17</v>
-      </c>
       <c r="L6" s="1">
-        <v>8.9600000000000009</v>
+        <v>9.36</v>
       </c>
       <c r="M6" s="1">
-        <v>3.26</v>
+        <v>3.51</v>
       </c>
       <c r="N6" s="1">
-        <v>9.36</v>
+        <v>9.8699999999999992</v>
       </c>
       <c r="O6" s="1">
-        <v>3.51</v>
+        <v>3.96</v>
       </c>
       <c r="P6" s="1">
-        <v>9.8699999999999992</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>3.96</v>
-      </c>
-      <c r="R6" s="1">
         <v>7.91</v>
       </c>
       <c r="U6">
@@ -6621,45 +4911,39 @@
         <v>1.85</v>
       </c>
       <c r="E7" s="1">
-        <v>3.27</v>
+        <v>3.25</v>
       </c>
       <c r="F7" s="1">
-        <v>2.89</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="G7" s="1">
-        <v>3.25</v>
+        <v>3.47</v>
       </c>
       <c r="H7" s="1">
-        <v>2.4500000000000002</v>
+        <v>6.14</v>
       </c>
       <c r="I7" s="1">
-        <v>3.47</v>
+        <v>3.04</v>
       </c>
       <c r="J7" s="1">
-        <v>6.14</v>
+        <v>9.0299999999999994</v>
       </c>
       <c r="K7" s="1">
-        <v>3.04</v>
+        <v>3.51</v>
       </c>
       <c r="L7" s="1">
-        <v>9.0299999999999994</v>
+        <v>9.39</v>
       </c>
       <c r="M7" s="1">
-        <v>3.51</v>
+        <v>3.71</v>
       </c>
       <c r="N7" s="1">
-        <v>9.39</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="O7" s="1">
-        <v>3.71</v>
+        <v>4.08</v>
       </c>
       <c r="P7" s="1">
-        <v>9.8800000000000008</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>4.08</v>
-      </c>
-      <c r="R7" s="1">
         <v>8.18</v>
       </c>
       <c r="U7">
@@ -6713,40 +4997,40 @@
         <v>1.68</v>
       </c>
       <c r="E8" s="1">
-        <v>3.34</v>
+        <v>3.3</v>
       </c>
       <c r="F8" s="1">
-        <v>3.36</v>
+        <v>3.12</v>
       </c>
       <c r="G8" s="1">
-        <v>3.3</v>
+        <v>3.37</v>
       </c>
       <c r="H8" s="1">
-        <v>3.12</v>
+        <v>5.81</v>
       </c>
       <c r="I8" s="1">
-        <v>3.37</v>
+        <v>2.95</v>
       </c>
       <c r="J8" s="1">
-        <v>5.81</v>
+        <v>9.1</v>
       </c>
       <c r="K8" s="1">
-        <v>2.95</v>
+        <v>3.68</v>
       </c>
       <c r="L8" s="1">
-        <v>9.1</v>
+        <v>9.44</v>
       </c>
       <c r="M8" s="1">
-        <v>3.68</v>
+        <v>3.9</v>
       </c>
       <c r="N8" s="1">
-        <v>9.44</v>
-      </c>
-      <c r="O8" s="1">
-        <v>3.9</v>
-      </c>
-      <c r="P8" s="1">
         <v>9.8800000000000008</v>
+      </c>
+      <c r="O8" s="5">
+        <v>3.55</v>
+      </c>
+      <c r="P8" s="5">
+        <v>3.42</v>
       </c>
       <c r="U8">
         <v>1.81</v>
@@ -6798,29 +5082,35 @@
       <c r="D9" s="1">
         <v>0.91</v>
       </c>
+      <c r="E9" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3.64</v>
+      </c>
       <c r="G9" s="1">
-        <v>3.35</v>
+        <v>3.6</v>
       </c>
       <c r="H9" s="1">
-        <v>3.64</v>
-      </c>
-      <c r="I9" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="J9" s="1">
         <v>6.97</v>
       </c>
+      <c r="K9" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="L9" s="1">
+        <v>9.44</v>
+      </c>
       <c r="M9" s="1">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="N9" s="1">
-        <v>9.44</v>
-      </c>
-      <c r="O9" s="1">
-        <v>4</v>
-      </c>
-      <c r="P9" s="1">
         <v>9.8800000000000008</v>
+      </c>
+      <c r="O9" s="5">
+        <v>3.59</v>
+      </c>
+      <c r="P9" s="5">
+        <v>4.1900000000000004</v>
       </c>
       <c r="U9">
         <v>1.76</v>
@@ -6872,22 +5162,22 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="G10" s="1">
+      <c r="E10" s="1">
         <v>3.49</v>
       </c>
-      <c r="H10" s="1">
+      <c r="F10" s="1">
         <v>3.12</v>
       </c>
+      <c r="K10" s="1">
+        <v>4.03</v>
+      </c>
+      <c r="L10" s="1">
+        <v>9.44</v>
+      </c>
       <c r="M10" s="1">
-        <v>4.03</v>
+        <v>4.21</v>
       </c>
       <c r="N10" s="1">
-        <v>9.44</v>
-      </c>
-      <c r="O10" s="1">
-        <v>4.21</v>
-      </c>
-      <c r="P10" s="1">
         <v>9.8800000000000008</v>
       </c>
       <c r="U10">
@@ -6940,11 +5230,11 @@
       <c r="D11" s="1">
         <v>1.65</v>
       </c>
-      <c r="G11" s="1">
-        <v>3.55</v>
-      </c>
-      <c r="H11" s="1">
-        <v>3.42</v>
+      <c r="E11" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.84</v>
       </c>
       <c r="U11">
         <v>1.67</v>
@@ -6990,11 +5280,11 @@
       </c>
     </row>
     <row r="12" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="G12" s="1">
-        <v>3.59</v>
-      </c>
-      <c r="H12" s="1">
-        <v>4.1900000000000004</v>
+      <c r="E12" s="1">
+        <v>3.18</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.48</v>
       </c>
       <c r="U12">
         <v>1.62</v>
@@ -7040,11 +5330,11 @@
       </c>
     </row>
     <row r="13" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="G13" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2.84</v>
+      <c r="E13" s="1">
+        <v>3.07</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
       </c>
       <c r="U13">
         <v>1.57</v>
@@ -7090,6 +5380,12 @@
       </c>
     </row>
     <row r="14" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <v>3.12</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.73</v>
+      </c>
       <c r="U14">
         <v>1.52</v>
       </c>
@@ -7134,8 +5430,11 @@
       </c>
     </row>
     <row r="15" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>31</v>
+      <c r="E15" s="1">
+        <v>3.23</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2.48</v>
       </c>
       <c r="U15">
         <v>1.47</v>
@@ -7181,32 +5480,11 @@
       </c>
     </row>
     <row r="16" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>7</v>
+      <c r="E16" s="1">
+        <v>3.27</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.89</v>
       </c>
       <c r="U16">
         <v>1.42</v>
@@ -7252,59 +5530,11 @@
       </c>
     </row>
     <row r="17" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>27</v>
+      <c r="E17" s="1">
+        <v>3.34</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3.36</v>
       </c>
       <c r="U17">
         <v>1.37</v>
@@ -7350,77 +5580,11 @@
       </c>
     </row>
     <row r="18" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <f>$B$47-A3</f>
-        <v>1.3000000000000003</v>
-      </c>
-      <c r="B18" s="1">
-        <f>$B$46-B3</f>
-        <v>10</v>
-      </c>
-      <c r="C18" s="1">
-        <f>$B$47-C3</f>
-        <v>1.27</v>
-      </c>
-      <c r="D18" s="1">
-        <f>$B$46-D3</f>
-        <v>7.93</v>
-      </c>
       <c r="E18" s="1">
-        <f>$B$47-E3</f>
-        <v>1.52</v>
+        <v>3.27</v>
       </c>
       <c r="F18" s="1">
-        <f>$B$46-F3</f>
-        <v>7.52</v>
-      </c>
-      <c r="G18" s="1">
-        <f>$B$47-G3</f>
-        <v>1.6400000000000001</v>
-      </c>
-      <c r="H18" s="1">
-        <f>$B$46-H3</f>
-        <v>10</v>
-      </c>
-      <c r="I18" s="1">
-        <f>$B$47-I3</f>
-        <v>1.7000000000000002</v>
-      </c>
-      <c r="J18" s="1">
-        <f>$B$46-J3</f>
-        <v>10</v>
-      </c>
-      <c r="K18" s="1">
-        <f>$B$47-K3</f>
-        <v>1.46</v>
-      </c>
-      <c r="L18" s="1">
-        <f>$B$46-L3</f>
-        <v>1.1400000000000006</v>
-      </c>
-      <c r="M18" s="1">
-        <f>$B$47-M3</f>
-        <v>1.75</v>
-      </c>
-      <c r="N18" s="1">
-        <f>$B$46-N3</f>
-        <v>0.74000000000000021</v>
-      </c>
-      <c r="O18" s="1">
-        <f>$B$47-O3</f>
-        <v>1.7000000000000002</v>
-      </c>
-      <c r="P18" s="1">
-        <f>$B$46-P3</f>
-        <v>0.11999999999999922</v>
-      </c>
-      <c r="Q18" s="1">
-        <f>$B$47-Q3</f>
-        <v>1.0500000000000003</v>
-      </c>
-      <c r="R18" s="1">
-        <f>$B$46-R3</f>
-        <v>4.5999999999999996</v>
+        <v>2.89</v>
       </c>
       <c r="W18">
         <v>1.47</v>
@@ -7460,77 +5624,11 @@
       </c>
     </row>
     <row r="19" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <f t="shared" ref="A19:A22" si="0">$B$47-A4</f>
-        <v>1.27</v>
-      </c>
-      <c r="B19" s="1">
-        <f t="shared" ref="B19:B21" si="1">$B$46-B4</f>
-        <v>9.15</v>
-      </c>
-      <c r="C19" s="1">
-        <f t="shared" ref="C19:C26" si="2">$B$47-C4</f>
-        <v>1.2400000000000002</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" ref="D19:D26" si="3">$B$46-D4</f>
-        <v>7.76</v>
-      </c>
       <c r="E19" s="1">
-        <f t="shared" ref="E19:E23" si="4">$B$47-E4</f>
-        <v>1.6300000000000003</v>
+        <v>3.34</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" ref="F19:F24" si="5">$B$46-F4</f>
-        <v>10</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" ref="G19:G28" si="6">$B$47-G4</f>
-        <v>1.58</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" ref="H19:H29" si="7">$B$46-H4</f>
-        <v>8.98</v>
-      </c>
-      <c r="I19" s="1">
-        <f t="shared" ref="I19:I25" si="8">$B$47-I4</f>
-        <v>1.6100000000000003</v>
-      </c>
-      <c r="J19" s="1">
-        <f t="shared" ref="J19:J24" si="9">$B$46-J4</f>
-        <v>7.1099999999999994</v>
-      </c>
-      <c r="K19" s="1">
-        <f t="shared" ref="K19:K25" si="10">$B$47-K4</f>
-        <v>1.1700000000000004</v>
-      </c>
-      <c r="L19" s="1">
-        <f t="shared" ref="L19:L23" si="11">$B$46-L4</f>
-        <v>1.2899999999999991</v>
-      </c>
-      <c r="M19" s="1">
-        <f t="shared" ref="M19:M25" si="12">$B$47-M4</f>
-        <v>1.6400000000000001</v>
-      </c>
-      <c r="N19" s="1">
-        <f t="shared" ref="N19:N25" si="13">$B$46-N4</f>
-        <v>0.66999999999999993</v>
-      </c>
-      <c r="O19" s="1">
-        <f t="shared" ref="O19:O25" si="14">$B$47-O4</f>
-        <v>1.6</v>
-      </c>
-      <c r="P19" s="1">
-        <f t="shared" ref="P19:P25" si="15">$B$46-P4</f>
-        <v>0.11999999999999922</v>
-      </c>
-      <c r="Q19" s="1">
-        <f t="shared" ref="Q19:Q22" si="16">$B$47-Q4</f>
-        <v>0.95000000000000018</v>
-      </c>
-      <c r="R19" s="1">
-        <f t="shared" ref="R19:R22" si="17">$B$46-R4</f>
-        <v>3.17</v>
+        <v>3.36</v>
       </c>
       <c r="W19">
         <v>1.42</v>
@@ -7570,78 +5668,6 @@
       </c>
     </row>
     <row r="20" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2400000000000002</v>
-      </c>
-      <c r="B20" s="1">
-        <f t="shared" si="1"/>
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="C20" s="1">
-        <f t="shared" si="2"/>
-        <v>1.31</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" si="3"/>
-        <v>7.66</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="4"/>
-        <v>1.58</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" si="5"/>
-        <v>9.27</v>
-      </c>
-      <c r="G20" s="1">
-        <f t="shared" si="6"/>
-        <v>1.5500000000000003</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" si="7"/>
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="I20" s="1">
-        <f t="shared" si="8"/>
-        <v>1.5300000000000002</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="9"/>
-        <v>6.74</v>
-      </c>
-      <c r="K20" s="1">
-        <f t="shared" si="10"/>
-        <v>1.35</v>
-      </c>
-      <c r="L20" s="1">
-        <f t="shared" si="11"/>
-        <v>1.3399999999999999</v>
-      </c>
-      <c r="M20" s="1">
-        <f t="shared" si="12"/>
-        <v>1.52</v>
-      </c>
-      <c r="N20" s="1">
-        <f t="shared" si="13"/>
-        <v>0.66000000000000014</v>
-      </c>
-      <c r="O20" s="1">
-        <f t="shared" si="14"/>
-        <v>1.4000000000000004</v>
-      </c>
-      <c r="P20" s="1">
-        <f t="shared" si="15"/>
-        <v>0.11999999999999922</v>
-      </c>
-      <c r="Q20" s="1">
-        <f t="shared" si="16"/>
-        <v>0.8400000000000003</v>
-      </c>
-      <c r="R20" s="1">
-        <f t="shared" si="17"/>
-        <v>3</v>
-      </c>
       <c r="W20">
         <v>1.37</v>
       </c>
@@ -7674,78 +5700,6 @@
       </c>
     </row>
     <row r="21" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2200000000000002</v>
-      </c>
-      <c r="B21" s="1">
-        <f t="shared" si="1"/>
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="C21" s="1">
-        <f t="shared" si="2"/>
-        <v>1.3800000000000003</v>
-      </c>
-      <c r="D21" s="1">
-        <f t="shared" si="3"/>
-        <v>7.8</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="4"/>
-        <v>1.4700000000000002</v>
-      </c>
-      <c r="F21" s="1">
-        <f t="shared" si="5"/>
-        <v>7.52</v>
-      </c>
-      <c r="G21" s="1">
-        <f t="shared" si="6"/>
-        <v>1.5</v>
-      </c>
-      <c r="H21" s="1">
-        <f t="shared" si="7"/>
-        <v>7.75</v>
-      </c>
-      <c r="I21" s="1">
-        <f t="shared" si="8"/>
-        <v>1.4400000000000004</v>
-      </c>
-      <c r="J21" s="1">
-        <f t="shared" si="9"/>
-        <v>5.55</v>
-      </c>
-      <c r="K21" s="1">
-        <f t="shared" si="10"/>
-        <v>1.5300000000000002</v>
-      </c>
-      <c r="L21" s="1">
-        <f t="shared" si="11"/>
-        <v>1.0399999999999991</v>
-      </c>
-      <c r="M21" s="1">
-        <f t="shared" si="12"/>
-        <v>1.4400000000000004</v>
-      </c>
-      <c r="N21" s="1">
-        <f t="shared" si="13"/>
-        <v>0.64000000000000057</v>
-      </c>
-      <c r="O21" s="1">
-        <f t="shared" si="14"/>
-        <v>1.1900000000000004</v>
-      </c>
-      <c r="P21" s="1">
-        <f t="shared" si="15"/>
-        <v>0.13000000000000078</v>
-      </c>
-      <c r="Q21" s="1">
-        <f t="shared" si="16"/>
-        <v>0.74000000000000021</v>
-      </c>
-      <c r="R21" s="1">
-        <f t="shared" si="17"/>
-        <v>2.09</v>
-      </c>
       <c r="AA21">
         <v>1.27</v>
       </c>
@@ -7760,70 +5714,8 @@
       </c>
     </row>
     <row r="22" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="C22" s="1">
-        <f t="shared" si="2"/>
-        <v>1.4500000000000002</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="3"/>
-        <v>8.15</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="4"/>
-        <v>1.4300000000000002</v>
-      </c>
-      <c r="F22" s="1">
-        <f t="shared" si="5"/>
-        <v>7.1099999999999994</v>
-      </c>
-      <c r="G22" s="1">
-        <f t="shared" si="6"/>
-        <v>1.4500000000000002</v>
-      </c>
-      <c r="H22" s="1">
-        <f t="shared" si="7"/>
-        <v>7.55</v>
-      </c>
-      <c r="I22" s="1">
-        <f t="shared" si="8"/>
-        <v>1.23</v>
-      </c>
-      <c r="J22" s="1">
-        <f t="shared" si="9"/>
-        <v>3.8600000000000003</v>
-      </c>
-      <c r="K22" s="1">
-        <f t="shared" si="10"/>
-        <v>1.6600000000000001</v>
-      </c>
-      <c r="L22" s="1">
-        <f t="shared" si="11"/>
-        <v>0.97000000000000064</v>
-      </c>
-      <c r="M22" s="1">
-        <f t="shared" si="12"/>
-        <v>1.1900000000000004</v>
-      </c>
-      <c r="N22" s="1">
-        <f t="shared" si="13"/>
-        <v>0.60999999999999943</v>
-      </c>
-      <c r="O22" s="1">
-        <f t="shared" si="14"/>
-        <v>0.99000000000000021</v>
-      </c>
-      <c r="P22" s="1">
-        <f t="shared" si="15"/>
-        <v>0.11999999999999922</v>
-      </c>
-      <c r="Q22" s="1">
-        <f t="shared" si="16"/>
-        <v>0.62000000000000011</v>
-      </c>
-      <c r="R22" s="1">
-        <f t="shared" si="17"/>
-        <v>1.8200000000000003</v>
+      <c r="A22" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="AA22">
         <v>1.23</v>
@@ -7833,63 +5725,17 @@
       </c>
     </row>
     <row r="23" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="C23" s="1">
-        <f t="shared" si="2"/>
-        <v>1.48</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="3"/>
-        <v>8.32</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" si="4"/>
-        <v>1.3600000000000003</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="5"/>
-        <v>6.6400000000000006</v>
-      </c>
-      <c r="G23" s="1">
-        <f t="shared" si="6"/>
-        <v>1.4000000000000004</v>
-      </c>
-      <c r="H23" s="1">
-        <f t="shared" si="7"/>
-        <v>6.88</v>
-      </c>
-      <c r="I23" s="1">
-        <f t="shared" si="8"/>
-        <v>1.33</v>
-      </c>
-      <c r="J23" s="1">
-        <f t="shared" si="9"/>
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="K23" s="1">
-        <f t="shared" si="10"/>
-        <v>1.75</v>
-      </c>
-      <c r="L23" s="1">
-        <f t="shared" si="11"/>
-        <v>0.90000000000000036</v>
-      </c>
-      <c r="M23" s="1">
-        <f t="shared" si="12"/>
-        <v>1.02</v>
-      </c>
-      <c r="N23" s="1">
-        <f t="shared" si="13"/>
-        <v>0.5600000000000005</v>
-      </c>
-      <c r="O23" s="1">
-        <f t="shared" si="14"/>
-        <v>0.80000000000000027</v>
-      </c>
-      <c r="P23" s="1">
-        <f t="shared" si="15"/>
-        <v>0.11999999999999922</v>
-      </c>
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="Q23" s="1"/>
       <c r="AA23">
         <v>1.18</v>
       </c>
@@ -7898,49 +5744,25 @@
       </c>
     </row>
     <row r="24" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="C24" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5500000000000003</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" si="3"/>
-        <v>9.09</v>
-      </c>
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1">
-        <f t="shared" si="6"/>
-        <v>1.35</v>
-      </c>
-      <c r="H24" s="1">
-        <f t="shared" si="7"/>
-        <v>6.3599999999999994</v>
-      </c>
-      <c r="I24" s="1">
-        <f t="shared" si="8"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J24" s="1">
-        <f t="shared" si="9"/>
-        <v>3.0300000000000002</v>
-      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="M24" s="1">
-        <f t="shared" si="12"/>
-        <v>0.80000000000000027</v>
-      </c>
-      <c r="N24" s="1">
-        <f t="shared" si="13"/>
-        <v>0.5600000000000005</v>
-      </c>
-      <c r="O24" s="1">
-        <f t="shared" si="14"/>
-        <v>0.70000000000000018</v>
-      </c>
-      <c r="P24" s="1">
-        <f t="shared" si="15"/>
-        <v>0.11999999999999922</v>
-      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
       <c r="AA24">
         <v>1.1299999999999999</v>
       </c>
@@ -7949,41 +5771,23 @@
       </c>
     </row>
     <row r="25" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="C25" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5700000000000003</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" si="6"/>
-        <v>1.21</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" si="7"/>
-        <v>6.88</v>
-      </c>
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
       <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="M25" s="1">
-        <f t="shared" si="12"/>
-        <v>0.66999999999999993</v>
-      </c>
-      <c r="N25" s="1">
-        <f t="shared" si="13"/>
-        <v>0.5600000000000005</v>
-      </c>
-      <c r="O25" s="1">
-        <f t="shared" si="14"/>
-        <v>0.49000000000000021</v>
-      </c>
-      <c r="P25" s="1">
-        <f t="shared" si="15"/>
-        <v>0.11999999999999922</v>
-      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
       <c r="AA25">
         <v>1.08</v>
       </c>
@@ -7992,23 +5796,23 @@
       </c>
     </row>
     <row r="26" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="C26" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5100000000000002</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="3"/>
-        <v>8.35</v>
-      </c>
-      <c r="G26" s="1">
-        <f t="shared" si="6"/>
-        <v>1.1500000000000004</v>
-      </c>
-      <c r="H26" s="1">
-        <f>$B$46-H11</f>
-        <v>6.58</v>
-      </c>
+      <c r="A26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
       <c r="AA26">
         <v>1.03</v>
       </c>
@@ -8017,15 +5821,20 @@
       </c>
     </row>
     <row r="27" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="G27" s="1">
-        <f t="shared" si="6"/>
-        <v>1.1100000000000003</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" si="7"/>
-        <v>5.81</v>
-      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
       <c r="AA27">
         <v>0.98</v>
       </c>
@@ -8034,15 +5843,20 @@
       </c>
     </row>
     <row r="28" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="G28" s="1">
-        <f t="shared" si="6"/>
-        <v>1.3000000000000003</v>
-      </c>
-      <c r="H28" s="1">
-        <f t="shared" si="7"/>
-        <v>7.16</v>
-      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
       <c r="AA28">
         <v>0.88</v>
       </c>
@@ -8050,8 +5864,27 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H29" s="1"/>
+    <row r="29" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
       <c r="AA29">
         <v>0.84</v>
       </c>
@@ -8059,13 +5892,25 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>51</v>
-      </c>
-      <c r="P30" t="s">
-        <v>50</v>
-      </c>
+    <row r="30" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
       <c r="AA30">
         <v>0.79</v>
       </c>
@@ -8074,6 +5919,17 @@
       </c>
     </row>
     <row r="31" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
       <c r="AA31">
         <v>0.74</v>
       </c>
@@ -8081,129 +5937,121 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="3">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50">
+    <row r="32" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
         <f>1/2250</f>
         <v>4.4444444444444447E-4</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
         <f>1/-226</f>
         <v>-4.4247787610619468E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52">
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
         <v>8.68</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53">
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
         <f>10/10^9</f>
         <v>1E-8</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>37</v>
-      </c>
-      <c r="B54">
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
         <f>100/10^9</f>
         <v>9.9999999999999995E-8</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <f>B37</f>
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <f>B37/B36</f>
+        <v>10</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B55">
-        <f>B54</f>
-        <v>9.9999999999999995E-8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B41">
+        <f>B33/B34</f>
+        <v>-0.10044444444444445</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B57">
-        <f>B54/B53</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>40</v>
-      </c>
-      <c r="B58">
-        <f>B50/B51</f>
-        <v>-0.10044444444444445</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>41</v>
-      </c>
-      <c r="B59">
-        <f>100*1000*B55/3300</f>
+      <c r="B42">
+        <f>100*1000*B38/3300</f>
         <v>3.0303030303030305E-6</v>
       </c>
     </row>
@@ -8228,40 +6076,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8299,11 +6147,11 @@
         <v>3</v>
       </c>
       <c r="K2">
-        <f>'Состояние системы'!$B$47 - A2</f>
+        <f>'Состояние системы'!$B$30 - A2</f>
         <v>1.2800000000000002</v>
       </c>
       <c r="L2">
-        <f>'Состояние системы'!$B$46-B2</f>
+        <f>'Состояние системы'!$B$29-B2</f>
         <v>7.82</v>
       </c>
     </row>
@@ -8342,11 +6190,11 @@
         <v>4</v>
       </c>
       <c r="K3">
-        <f>'Состояние системы'!$B$47 - A3</f>
+        <f>'Состояние системы'!$B$30 - A3</f>
         <v>1.3600000000000003</v>
       </c>
       <c r="L3">
-        <f>'Состояние системы'!$B$46-B3</f>
+        <f>'Состояние системы'!$B$29-B3</f>
         <v>7.8100000000000005</v>
       </c>
     </row>
@@ -8385,11 +6233,11 @@
         <v>6.5</v>
       </c>
       <c r="K4">
-        <f>'Состояние системы'!$B$47 - A4</f>
+        <f>'Состояние системы'!$B$30 - A4</f>
         <v>1.4700000000000002</v>
       </c>
       <c r="L4">
-        <f>'Состояние системы'!$B$46-B4</f>
+        <f>'Состояние системы'!$B$29-B4</f>
         <v>8.32</v>
       </c>
     </row>
@@ -8428,11 +6276,11 @@
         <v>5.5</v>
       </c>
       <c r="K5">
-        <f>'Состояние системы'!$B$47 - A5</f>
+        <f>'Состояние системы'!$B$30 - A5</f>
         <v>1.5100000000000002</v>
       </c>
       <c r="L5">
-        <f>'Состояние системы'!$B$46-B5</f>
+        <f>'Состояние системы'!$B$29-B5</f>
         <v>10</v>
       </c>
     </row>
@@ -8471,11 +6319,11 @@
         <v>6.5</v>
       </c>
       <c r="K6">
-        <f>'Состояние системы'!$B$47 - A6</f>
+        <f>'Состояние системы'!$B$30 - A6</f>
         <v>1.5700000000000003</v>
       </c>
       <c r="L6">
-        <f>'Состояние системы'!$B$46-B6</f>
+        <f>'Состояние системы'!$B$29-B6</f>
         <v>10</v>
       </c>
     </row>
@@ -8514,11 +6362,11 @@
         <v>4</v>
       </c>
       <c r="K7">
-        <f>'Состояние системы'!$B$47 - A7</f>
+        <f>'Состояние системы'!$B$30 - A7</f>
         <v>1.35</v>
       </c>
       <c r="L7">
-        <f>'Состояние системы'!$B$46-B7</f>
+        <f>'Состояние системы'!$B$29-B7</f>
         <v>9.14</v>
       </c>
     </row>
@@ -8557,11 +6405,11 @@
         <v>2.6</v>
       </c>
       <c r="K8">
-        <f>'Состояние системы'!$B$47 - A8</f>
+        <f>'Состояние системы'!$B$30 - A8</f>
         <v>1.2000000000000002</v>
       </c>
       <c r="L8">
-        <f>'Состояние системы'!$B$46-B8</f>
+        <f>'Состояние системы'!$B$29-B8</f>
         <v>8.14</v>
       </c>
     </row>
@@ -8600,11 +6448,11 @@
         <v>4</v>
       </c>
       <c r="K9">
-        <f>'Состояние системы'!$B$47 - A9</f>
+        <f>'Состояние системы'!$B$30 - A9</f>
         <v>1.37</v>
       </c>
       <c r="L9">
-        <f>'Состояние системы'!$B$46-B9</f>
+        <f>'Состояние системы'!$B$29-B9</f>
         <v>10</v>
       </c>
     </row>
@@ -8643,11 +6491,11 @@
         <v>5.8</v>
       </c>
       <c r="K10">
-        <f>'Состояние системы'!$B$47 - A10</f>
+        <f>'Состояние системы'!$B$30 - A10</f>
         <v>1.5500000000000003</v>
       </c>
       <c r="L10">
-        <f>'Состояние системы'!$B$46-B10</f>
+        <f>'Состояние системы'!$B$29-B10</f>
         <v>8.69</v>
       </c>
     </row>
@@ -8686,11 +6534,11 @@
         <v>5.8</v>
       </c>
       <c r="K11">
-        <f>'Состояние системы'!$B$47 - A11</f>
+        <f>'Состояние системы'!$B$30 - A11</f>
         <v>1.5500000000000003</v>
       </c>
       <c r="L11">
-        <f>'Состояние системы'!$B$46-B11</f>
+        <f>'Состояние системы'!$B$29-B11</f>
         <v>9.44</v>
       </c>
     </row>
@@ -8729,11 +6577,11 @@
         <v>4.8</v>
       </c>
       <c r="K12">
-        <f>'Состояние системы'!$B$47 - A12</f>
+        <f>'Состояние системы'!$B$30 - A12</f>
         <v>1.4400000000000004</v>
       </c>
       <c r="L12">
-        <f>'Состояние системы'!$B$46-B12</f>
+        <f>'Состояние системы'!$B$29-B12</f>
         <v>10</v>
       </c>
     </row>
@@ -8772,11 +6620,11 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="K13">
-        <f>'Состояние системы'!$B$47 - A13</f>
+        <f>'Состояние системы'!$B$30 - A13</f>
         <v>1.4400000000000004</v>
       </c>
       <c r="L13">
-        <f>'Состояние системы'!$B$46-B13</f>
+        <f>'Состояние системы'!$B$29-B13</f>
         <v>9.16</v>
       </c>
     </row>
@@ -8815,11 +6663,11 @@
         <v>4</v>
       </c>
       <c r="K14">
-        <f>'Состояние системы'!$B$47 - A14</f>
+        <f>'Состояние системы'!$B$30 - A14</f>
         <v>1.31</v>
       </c>
       <c r="L14">
-        <f>'Состояние системы'!$B$46-B14</f>
+        <f>'Состояние системы'!$B$29-B14</f>
         <v>10</v>
       </c>
     </row>
@@ -8858,11 +6706,11 @@
         <v>3.8</v>
       </c>
       <c r="K15">
-        <f>'Состояние системы'!$B$47 - A15</f>
+        <f>'Состояние системы'!$B$30 - A15</f>
         <v>1.31</v>
       </c>
       <c r="L15">
-        <f>'Состояние системы'!$B$46-B15</f>
+        <f>'Состояние системы'!$B$29-B15</f>
         <v>7.93</v>
       </c>
     </row>
@@ -8901,11 +6749,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="K16">
-        <f>'Состояние системы'!$B$47 - A16</f>
+        <f>'Состояние системы'!$B$30 - A16</f>
         <v>1.1500000000000004</v>
       </c>
       <c r="L16">
-        <f>'Состояние системы'!$B$46-B16</f>
+        <f>'Состояние системы'!$B$29-B16</f>
         <v>8.27</v>
       </c>
     </row>
@@ -8930,37 +6778,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8991,11 +6839,11 @@
         <v>3</v>
       </c>
       <c r="I2">
-        <f>'Состояние системы'!$B$46 - B2</f>
+        <f>'Состояние системы'!$B$29 - B2</f>
         <v>10</v>
       </c>
       <c r="J2">
-        <f>'Состояние системы'!$B$47-A2</f>
+        <f>'Состояние системы'!$B$30-A2</f>
         <v>1.5500000000000003</v>
       </c>
       <c r="K2">
@@ -9029,7 +6877,7 @@
         <v>2.5</v>
       </c>
       <c r="I3">
-        <f>'Состояние системы'!$B$46 - B3</f>
+        <f>'Состояние системы'!$B$29 - B3</f>
         <v>8.8000000000000007</v>
       </c>
       <c r="K3">
@@ -9063,7 +6911,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f>'Состояние системы'!$B$46 - B4</f>
+        <f>'Состояние системы'!$B$29 - B4</f>
         <v>7.9</v>
       </c>
       <c r="K4">
@@ -9097,7 +6945,7 @@
         <v>0.5</v>
       </c>
       <c r="I5">
-        <f>'Состояние системы'!$B$46 - B5</f>
+        <f>'Состояние системы'!$B$29 - B5</f>
         <v>7.15</v>
       </c>
       <c r="K5">
@@ -9131,7 +6979,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <f>'Состояние системы'!$B$46 - B6</f>
+        <f>'Состояние системы'!$B$29 - B6</f>
         <v>7.1400000000000006</v>
       </c>
       <c r="K6">
@@ -9165,7 +7013,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <f>'Состояние системы'!$B$46 - B7</f>
+        <f>'Состояние системы'!$B$29 - B7</f>
         <v>1.08</v>
       </c>
       <c r="K7">
@@ -9199,7 +7047,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <f>'Состояние системы'!$B$46 - B8</f>
+        <f>'Состояние системы'!$B$29 - B8</f>
         <v>1.0700000000000003</v>
       </c>
       <c r="K8">
@@ -9233,7 +7081,7 @@
         <v>0.5</v>
       </c>
       <c r="I9">
-        <f>'Состояние системы'!$B$46 - B9</f>
+        <f>'Состояние системы'!$B$29 - B9</f>
         <v>0.86999999999999922</v>
       </c>
       <c r="K9">
@@ -9267,7 +7115,7 @@
         <v>0.5</v>
       </c>
       <c r="I10">
-        <f>'Состояние системы'!$B$46 - B10</f>
+        <f>'Состояние системы'!$B$29 - B10</f>
         <v>0.83000000000000007</v>
       </c>
       <c r="K10">
@@ -9301,7 +7149,7 @@
         <v>0.75</v>
       </c>
       <c r="I11">
-        <f>'Состояние системы'!$B$46 - B11</f>
+        <f>'Состояние системы'!$B$29 - B11</f>
         <v>0.74000000000000021</v>
       </c>
       <c r="K11">
@@ -9335,7 +7183,7 @@
         <v>0.5</v>
       </c>
       <c r="I12">
-        <f>'Состояние системы'!$B$46 - B12</f>
+        <f>'Состояние системы'!$B$29 - B12</f>
         <v>0.69999999999999929</v>
       </c>
       <c r="K12">
@@ -9369,7 +7217,7 @@
         <v>3</v>
       </c>
       <c r="I13">
-        <f>'Состояние системы'!$B$46 - B13</f>
+        <f>'Состояние системы'!$B$29 - B13</f>
         <v>0.67999999999999972</v>
       </c>
       <c r="K13">
@@ -9403,7 +7251,7 @@
         <v>2</v>
       </c>
       <c r="I14">
-        <f>'Состояние системы'!$B$46 - B14</f>
+        <f>'Состояние системы'!$B$29 - B14</f>
         <v>0.36999999999999922</v>
       </c>
       <c r="K14">
@@ -9437,7 +7285,7 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <f>'Состояние системы'!$B$46 - B15</f>
+        <f>'Состояние системы'!$B$29 - B15</f>
         <v>0.22000000000000064</v>
       </c>
       <c r="K15">
@@ -9471,7 +7319,7 @@
         <v>0.4</v>
       </c>
       <c r="I16">
-        <f>'Состояние системы'!$B$46 - B16</f>
+        <f>'Состояние системы'!$B$29 - B16</f>
         <v>0.16999999999999993</v>
       </c>
       <c r="K16">
@@ -9505,7 +7353,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <f>'Состояние системы'!$B$46 - B17</f>
+        <f>'Состояние системы'!$B$29 - B17</f>
         <v>0.14000000000000057</v>
       </c>
       <c r="K17">
@@ -9534,13 +7382,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>